<commit_message>
Fixed up sankey and tableau for time
</commit_message>
<xml_diff>
--- a/visualizations/uber_day_of_week.xlsx
+++ b/visualizations/uber_day_of_week.xlsx
@@ -6,7 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2015" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2014" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2015" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,25 +20,25 @@
     <t>day_of_week</t>
   </si>
   <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
     <t>Sat</t>
   </si>
   <si>
-    <t>Fri</t>
-  </si>
-  <si>
-    <t>Thu</t>
+    <t>Mon</t>
   </si>
   <si>
     <t>Sun</t>
-  </si>
-  <si>
-    <t>Wed</t>
-  </si>
-  <si>
-    <t>Tue</t>
-  </si>
-  <si>
-    <t>Mon</t>
   </si>
 </sst>
 </file>
@@ -404,7 +405,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2414563</v>
+        <v>755145</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -412,7 +413,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2282571</v>
+        <v>741139</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -420,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2159598</v>
+        <v>696488</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -428,7 +429,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1952782</v>
+        <v>663789</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -436,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1893811</v>
+        <v>646114</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -444,12 +445,92 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1872902</v>
+        <v>541472</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>490180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2414563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2282571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2159598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1952782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1893811</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1872902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>1694252</v>

</xml_diff>